<commit_message>
almost done with radet and dqa
</commit_message>
<xml_diff>
--- a/DMP/Report/Template/DQA FY2017 Q3/DATIM PIVOT TABLE SAMPLE.xlsx
+++ b/DMP/Report/Template/DQA FY2017 Q3/DATIM PIVOT TABLE SAMPLE.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmadubuko\Google Drive\MGIC\Project\ShieldPortal\DMP\Report\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MGIC\DQA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6440"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13330"/>
   </bookViews>
   <sheets>
     <sheet name="data (13)" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" iterate="1" iterateCount="1" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>organisationunitid</t>
   </si>
@@ -27,22 +27,40 @@
     <t>organisationunitname</t>
   </si>
   <si>
-    <t>pmtct_art (n, dsd, newexistingart)</t>
-  </si>
-  <si>
-    <t>tx_curr (n, dsd)</t>
-  </si>
-  <si>
-    <t>ovc_hivstat (n, dsd, reportedstatus)</t>
-  </si>
-  <si>
-    <t>tb_art (n, dsd)</t>
+    <t>HTS_TST (N, DSD): HTS received results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMTCT_STAT (N, DSD, Age/KnownNewResult): Known Results </t>
+  </si>
+  <si>
+    <t>PMTCT_STAT (N, DSD, Age/KnownNewResult): Known Results, Known at Entry Positive</t>
+  </si>
+  <si>
+    <t>PMTCT_STAT (N, DSD, Age/KnownNewResult): Known Results, Newly Identified Positive</t>
+  </si>
+  <si>
+    <t>PMTCT_ART (N, DSD, NewExistingArt):ARVs</t>
+  </si>
+  <si>
+    <t>PMTCT_EID (N, DSD, Age/HIVStatus): Infant Testing</t>
+  </si>
+  <si>
+    <t>TX_CURR (N, DSD): Receiving ART</t>
+  </si>
+  <si>
+    <t>TX_NEW (N, DSD): New on ART</t>
+  </si>
+  <si>
+    <t>HTC _Only (excluding, PMTCT_STAT, TB_STAT, VMMC_CRC, PP_PRE, KP_PREV, OVC_HIVSTAT)</t>
+  </si>
+  <si>
+    <t>HTC_Only_Pos  (excluding positives from PMTCT_STAT, TB_STAT, VMMC_CRC, PP_PRE, KP_PREV, OVC_HIVSTAT)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -520,10 +538,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -569,8 +593,36 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -845,51 +897,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34" customWidth="1"/>
+    <col min="3" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="22.81640625" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" customWidth="1"/>
+    <col min="7" max="7" width="20.1796875" customWidth="1"/>
+    <col min="8" max="12" width="22.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="97.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="I1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B15" s="1"/>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>